<commit_message>
Adding report topics and profilling test.
</commit_message>
<xml_diff>
--- a/HarrisCornerDetection/Reports/Report.xlsx
+++ b/HarrisCornerDetection/Reports/Report.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Elapsed Nanoseconds</t>
   </si>
@@ -28,6 +28,36 @@
   </si>
   <si>
     <t>HarrisInputMatrix.txt</t>
+  </si>
+  <si>
+    <t>Optimized?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>Transformation performed</t>
+  </si>
+  <si>
+    <t>OrderStatisticsFiltering: find max</t>
+  </si>
+  <si>
+    <t>Elapsed Seconds</t>
+  </si>
+  <si>
+    <t>Matlab</t>
+  </si>
+  <si>
+    <t>Elapsed Milliseconds</t>
   </si>
 </sst>
 </file>
@@ -63,9 +93,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,32 +418,113 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="4" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
         <v>109174000</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" s="5">
+        <f>D2/10^6</f>
+        <v>109.17400000000001</v>
+      </c>
+      <c r="F2" s="4">
+        <f>D2/10^9</f>
+        <v>0.10917399999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D3" s="1">
+        <v>17294400</v>
+      </c>
+      <c r="E3" s="5">
+        <f>D3/10^6</f>
+        <v>17.2944</v>
+      </c>
+      <c r="F3" s="4">
+        <f>D3/10^9</f>
+        <v>1.7294400000000001E-2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <f>F4*10^9</f>
+        <v>61001062.393188402</v>
+      </c>
+      <c r="E4" s="5">
+        <f>D4/10^6</f>
+        <v>61.001062393188406</v>
+      </c>
+      <c r="F4">
+        <v>6.10010623931884E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>